<commit_message>
Complete logs for 14 week
</commit_message>
<xml_diff>
--- a/Logs/14th Week TeamLogs.xlsx
+++ b/Logs/14th Week TeamLogs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE0090E-B2E1-4F85-B961-A25D03E75C19}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C88F546-8217-492F-80F5-83276891896D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="24">
   <si>
     <t>Date</t>
   </si>
@@ -559,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -632,9 +632,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
@@ -654,12 +651,6 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -668,6 +659,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,23 +1051,23 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="64">
+      <c r="B8" s="61">
         <v>1</v>
       </c>
-      <c r="C8" s="65">
+      <c r="C8" s="62">
         <v>43584</v>
       </c>
-      <c r="D8" s="66">
+      <c r="D8" s="63">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E8" s="66">
+      <c r="E8" s="63">
         <v>0.72916666666666663</v>
       </c>
-      <c r="F8" s="58"/>
+      <c r="F8" s="55"/>
       <c r="G8" s="11">
         <v>90</v>
       </c>
-      <c r="H8" s="61" t="s">
+      <c r="H8" s="58" t="s">
         <v>19</v>
       </c>
       <c r="I8" s="20" t="s">
@@ -1080,23 +1077,23 @@
       <c r="K8" s="37"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="64">
+      <c r="B9" s="61">
         <v>2</v>
       </c>
-      <c r="C9" s="62">
+      <c r="C9" s="59">
         <v>43587</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="72">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E9" s="63">
+      <c r="E9" s="60">
         <v>0.47222222222222227</v>
       </c>
-      <c r="F9" s="59"/>
+      <c r="F9" s="56"/>
       <c r="G9" s="11">
         <v>80</v>
       </c>
-      <c r="H9" s="67" t="s">
+      <c r="H9" s="64" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="20" t="s">
@@ -1106,23 +1103,23 @@
       <c r="K9" s="38"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="64">
+      <c r="B10" s="61">
         <v>3</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="65">
         <v>43587</v>
       </c>
-      <c r="D10" s="63">
+      <c r="D10" s="60">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E10" s="63">
+      <c r="E10" s="60">
         <v>0.85416666666666663</v>
       </c>
-      <c r="F10" s="59"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="11">
         <v>90</v>
       </c>
-      <c r="H10" s="67" t="s">
+      <c r="H10" s="64" t="s">
         <v>17</v>
       </c>
       <c r="I10" s="20" t="s">
@@ -1132,23 +1129,23 @@
       <c r="K10" s="38"/>
     </row>
     <row r="11" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="64">
+      <c r="B11" s="61">
         <v>4</v>
       </c>
-      <c r="C11" s="62">
+      <c r="C11" s="59">
         <v>43588</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="60">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E11" s="63">
+      <c r="E11" s="60">
         <v>0.5</v>
       </c>
-      <c r="F11" s="59"/>
+      <c r="F11" s="56"/>
       <c r="G11" s="11">
         <v>240</v>
       </c>
-      <c r="H11" s="61" t="s">
+      <c r="H11" s="58" t="s">
         <v>19</v>
       </c>
       <c r="I11" s="20" t="s">
@@ -1158,21 +1155,21 @@
       <c r="K11" s="38"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="64"/>
-      <c r="C12" s="62">
+      <c r="B12" s="61"/>
+      <c r="C12" s="59">
         <v>43589</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="60">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E12" s="63">
+      <c r="E12" s="60">
         <v>0.72916666666666663</v>
       </c>
-      <c r="F12" s="61"/>
+      <c r="F12" s="58"/>
       <c r="G12" s="11">
         <v>180</v>
       </c>
-      <c r="H12" s="67" t="s">
+      <c r="H12" s="64" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="20"/>
@@ -1180,13 +1177,13 @@
       <c r="K12" s="38"/>
     </row>
     <row r="13" spans="2:11" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="64"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="61"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="58"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="61"/>
+      <c r="H13" s="58"/>
       <c r="I13" s="20"/>
       <c r="J13" s="4"/>
       <c r="K13" s="38"/>
@@ -1303,7 +1300,7 @@
   <dimension ref="B3:K22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1375,10 +1372,10 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="37.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
@@ -1405,162 +1402,162 @@
       </c>
     </row>
     <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="71">
+      <c r="B9" s="68">
         <v>1</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="69">
         <v>43584</v>
       </c>
-      <c r="D9" s="73">
+      <c r="D9" s="70">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E9" s="73">
+      <c r="E9" s="70">
         <v>0.72916666666666663</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="78">
+      <c r="F9" s="71"/>
+      <c r="G9" s="73">
         <f>(E9-D9)*24*60 - F9</f>
         <v>90</v>
       </c>
-      <c r="H9" s="74" t="s">
+      <c r="H9" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="74" t="s">
+      <c r="I9" s="71" t="s">
         <v>21</v>
       </c>
       <c r="J9" s="7"/>
       <c r="K9" s="44"/>
     </row>
     <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="70">
+      <c r="B10" s="67">
         <v>2</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="65">
         <v>43585</v>
       </c>
-      <c r="D10" s="69">
+      <c r="D10" s="66">
         <v>0.625</v>
       </c>
-      <c r="E10" s="69">
+      <c r="E10" s="66">
         <v>0.83333333333333337</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="79">
+      <c r="F10" s="64"/>
+      <c r="G10" s="74">
         <f t="shared" ref="G10:G14" si="0">(E10-D10)*24*60 - F10</f>
         <v>300.00000000000006</v>
       </c>
-      <c r="H10" s="67" t="s">
+      <c r="H10" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="74" t="s">
+      <c r="I10" s="71" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="40"/>
       <c r="K10" s="43"/>
     </row>
     <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="70">
+      <c r="B11" s="67">
         <v>3</v>
       </c>
-      <c r="C11" s="68">
+      <c r="C11" s="65">
         <v>43586</v>
       </c>
-      <c r="D11" s="69">
+      <c r="D11" s="66">
         <v>0.75</v>
       </c>
-      <c r="E11" s="80">
+      <c r="E11" s="75">
         <v>0.95833333333333337</v>
       </c>
       <c r="F11" s="46"/>
-      <c r="G11" s="81">
+      <c r="G11" s="76">
         <f t="shared" si="0"/>
         <v>300.00000000000006</v>
       </c>
       <c r="H11" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="82" t="s">
+      <c r="I11" s="77" t="s">
         <v>18</v>
       </c>
       <c r="J11" s="40"/>
       <c r="K11" s="43"/>
     </row>
     <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="60">
+      <c r="B12" s="57">
         <v>4</v>
       </c>
-      <c r="C12" s="83">
+      <c r="C12" s="78">
         <v>43587</v>
       </c>
-      <c r="D12" s="84">
+      <c r="D12" s="79">
         <v>0.5</v>
       </c>
-      <c r="E12" s="80">
+      <c r="E12" s="75">
         <v>0.70833333333333337</v>
       </c>
       <c r="F12" s="46"/>
-      <c r="G12" s="81">
+      <c r="G12" s="76">
         <f t="shared" si="0"/>
         <v>300.00000000000006</v>
       </c>
       <c r="H12" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="82" t="s">
+      <c r="I12" s="77" t="s">
         <v>18</v>
       </c>
       <c r="J12" s="40"/>
       <c r="K12" s="43"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="71">
+      <c r="B13" s="68">
         <v>5</v>
       </c>
-      <c r="C13" s="83">
+      <c r="C13" s="78">
         <v>43588</v>
       </c>
-      <c r="D13" s="84">
+      <c r="D13" s="79">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E13" s="69">
+      <c r="E13" s="66">
         <v>0.52083333333333337</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="79">
+      <c r="F13" s="64"/>
+      <c r="G13" s="74">
         <f t="shared" si="0"/>
         <v>270.00000000000011</v>
       </c>
-      <c r="H13" s="67" t="s">
+      <c r="H13" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="67" t="s">
+      <c r="I13" s="64" t="s">
         <v>23</v>
       </c>
       <c r="J13" s="40"/>
       <c r="K13" s="43"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="70">
+      <c r="B14" s="67">
         <v>6</v>
       </c>
-      <c r="C14" s="83">
+      <c r="C14" s="78">
         <v>43625</v>
       </c>
-      <c r="D14" s="84">
+      <c r="D14" s="79">
         <v>0.625</v>
       </c>
-      <c r="E14" s="69">
+      <c r="E14" s="66">
         <v>0.75</v>
       </c>
-      <c r="F14" s="67"/>
-      <c r="G14" s="79">
+      <c r="F14" s="64"/>
+      <c r="G14" s="74">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="H14" s="67" t="s">
+      <c r="H14" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="67" t="s">
+      <c r="I14" s="64" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="40"/>
@@ -1680,7 +1677,7 @@
   <dimension ref="B3:K22"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1753,10 +1750,10 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="34.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
@@ -1782,110 +1779,185 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="71"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="19"/>
+    <row r="9" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="68">
+        <v>1</v>
+      </c>
+      <c r="C9" s="69">
+        <v>43584</v>
+      </c>
+      <c r="D9" s="70">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E9" s="70">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F9" s="71"/>
+      <c r="G9" s="73">
+        <f>(E9-D9)*24*60 - F9</f>
+        <v>90</v>
+      </c>
+      <c r="H9" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="71" t="s">
+        <v>21</v>
+      </c>
       <c r="J9" s="49"/>
       <c r="K9" s="50"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="70"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="19"/>
+    <row r="10" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="67">
+        <v>2</v>
+      </c>
+      <c r="C10" s="65">
+        <v>43585</v>
+      </c>
+      <c r="D10" s="66">
+        <v>0.625</v>
+      </c>
+      <c r="E10" s="66">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F10" s="64"/>
+      <c r="G10" s="74">
+        <f t="shared" ref="G10:G13" si="0">(E10-D10)*24*60 - F10</f>
+        <v>300.00000000000006</v>
+      </c>
+      <c r="H10" s="64" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="71" t="s">
+        <v>18</v>
+      </c>
       <c r="J10" s="51"/>
       <c r="K10" s="52"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="70"/>
-      <c r="C11" s="68"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="19"/>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="67">
+        <v>3</v>
+      </c>
+      <c r="C11" s="65">
+        <v>43586</v>
+      </c>
+      <c r="D11" s="66">
+        <v>0.75</v>
+      </c>
+      <c r="E11" s="75">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="F11" s="46"/>
+      <c r="G11" s="76">
+        <f t="shared" si="0"/>
+        <v>300.00000000000006</v>
+      </c>
+      <c r="H11" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="77" t="s">
+        <v>18</v>
+      </c>
       <c r="J11" s="47"/>
       <c r="K11" s="48"/>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="70"/>
-      <c r="C12" s="68"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="67"/>
-      <c r="I12" s="19"/>
+    <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="57">
+        <v>4</v>
+      </c>
+      <c r="C12" s="78">
+        <v>43587</v>
+      </c>
+      <c r="D12" s="79">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="75">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F12" s="46"/>
+      <c r="G12" s="76">
+        <f t="shared" si="0"/>
+        <v>300.00000000000006</v>
+      </c>
+      <c r="H12" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="77" t="s">
+        <v>18</v>
+      </c>
       <c r="J12" s="47"/>
       <c r="K12" s="48"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="70"/>
-      <c r="C13" s="68"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="19"/>
+      <c r="B13" s="68">
+        <v>5</v>
+      </c>
+      <c r="C13" s="78">
+        <v>43588</v>
+      </c>
+      <c r="D13" s="79">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E13" s="66">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F13" s="64"/>
+      <c r="G13" s="74">
+        <f t="shared" si="0"/>
+        <v>270.00000000000011</v>
+      </c>
+      <c r="H13" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="64" t="s">
+        <v>23</v>
+      </c>
       <c r="J13" s="47"/>
       <c r="K13" s="48"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="70"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="67"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="64"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="67"/>
+      <c r="H14" s="64"/>
       <c r="I14" s="19"/>
       <c r="J14" s="47"/>
       <c r="K14" s="48"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="70"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="67"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="64"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="67"/>
+      <c r="H15" s="64"/>
       <c r="I15" s="19"/>
       <c r="J15" s="47"/>
       <c r="K15" s="48"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="70"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="67"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="64"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="67"/>
+      <c r="H16" s="64"/>
       <c r="I16" s="19"/>
       <c r="J16" s="4"/>
       <c r="K16" s="38"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="70"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="67"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="64"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="67"/>
+      <c r="H17" s="64"/>
       <c r="I17" s="19"/>
       <c r="J17" s="4"/>
       <c r="K17" s="38"/>
@@ -1948,7 +2020,7 @@
       </c>
       <c r="G22" s="17">
         <f>SUM(G9:G21)</f>
-        <v>0</v>
+        <v>1260.0000000000005</v>
       </c>
       <c r="H22" s="15"/>
       <c r="I22" s="15"/>
@@ -1965,10 +2037,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F48D277-4C33-425C-A628-D76A08925D5B}">
-  <dimension ref="B3:K19"/>
+  <dimension ref="B3:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,10 +2113,10 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="2:11" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="77"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
@@ -2071,49 +2143,49 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="70">
+      <c r="B9" s="67">
         <v>1</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="80">
         <v>43584</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="72">
         <v>0.66666666666666663</v>
       </c>
-      <c r="E9" s="73">
+      <c r="E9" s="70">
         <v>0.72916666666666663</v>
       </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="67">
+      <c r="F9" s="55"/>
+      <c r="G9" s="64">
         <f t="shared" ref="G9:G11" si="0">(E9-D9)*24*60 - F9</f>
         <v>90</v>
       </c>
-      <c r="H9" s="67" t="s">
+      <c r="H9" s="64" t="s">
         <v>19</v>
       </c>
       <c r="I9" s="19"/>
-      <c r="J9" s="57"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="53"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="60">
+      <c r="B10" s="57">
         <v>2</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="65">
         <v>43587</v>
       </c>
-      <c r="D10" s="75">
+      <c r="D10" s="72">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E10" s="69">
+      <c r="E10" s="66">
         <v>0.47222222222222227</v>
       </c>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67">
+      <c r="F10" s="64"/>
+      <c r="G10" s="64">
         <f t="shared" si="0"/>
         <v>80.000000000000028</v>
       </c>
-      <c r="H10" s="67" t="s">
+      <c r="H10" s="64" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="19"/>
@@ -2121,130 +2193,92 @@
       <c r="K10" s="53"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="70">
+      <c r="B11" s="67">
         <v>3</v>
       </c>
-      <c r="C11" s="68">
+      <c r="C11" s="65">
         <v>43587</v>
       </c>
-      <c r="D11" s="69">
+      <c r="D11" s="66">
         <v>0.79166666666666663</v>
       </c>
-      <c r="E11" s="69">
+      <c r="E11" s="66">
         <v>0.85416666666666663</v>
       </c>
-      <c r="F11" s="59"/>
-      <c r="G11" s="67">
+      <c r="F11" s="56"/>
+      <c r="G11" s="64">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="H11" s="67" t="s">
-        <v>18</v>
-      </c>
+      <c r="H11" s="64"/>
       <c r="I11" s="19"/>
       <c r="J11" s="53"/>
       <c r="K11" s="53"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="56"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="59"/>
+      <c r="B12" s="35"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="53"/>
+      <c r="H12" s="4"/>
       <c r="I12" s="19"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="38"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="56"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="53"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="38"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="56"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="53"/>
+      <c r="H14" s="4"/>
       <c r="I14" s="19"/>
       <c r="J14" s="4"/>
       <c r="K14" s="38"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="35"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="38"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="35"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="38"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="35"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="38"/>
-    </row>
-    <row r="18" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="36"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="39"/>
-    </row>
-    <row r="19" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="16" t="s">
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="36"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="39"/>
+    </row>
+    <row r="16" spans="2:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="17">
-        <f>SUM(G9:G18)</f>
+      <c r="G16" s="17">
+        <f>SUM(G9:G15)</f>
         <v>260</v>
       </c>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="18"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>